<commit_message>
addition of static and global variables
</commit_message>
<xml_diff>
--- a/Project_Grading_Rubric_Checklist.xlsx
+++ b/Project_Grading_Rubric_Checklist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjgly\Downloads\Spring 2024\AERSP 424\Final Project\AERSP424_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AERSP 424 Local\Project\AERSP424_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94053283-CABA-4249-A592-2E970AFCDF36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07501A3C-C1CD-454D-AD7B-69CAC61807CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{E08E36A2-DE9E-42A5-A6DD-8188537D7612}"/>
+    <workbookView xWindow="-27810" yWindow="7680" windowWidth="23280" windowHeight="13155" xr2:uid="{E08E36A2-DE9E-42A5-A6DD-8188537D7612}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -284,9 +284,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -324,7 +324,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -430,7 +430,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -572,7 +572,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -582,23 +582,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51F30247-08F3-4D53-8CE2-96A4DCDF6914}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="43.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.90625" customWidth="1"/>
-    <col min="5" max="5" width="255.54296875" customWidth="1"/>
+    <col min="1" max="1" width="43.64453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.87890625" customWidth="1"/>
+    <col min="5" max="5" width="255.52734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -615,7 +615,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -629,7 +629,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -643,7 +643,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -657,18 +657,21 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6">
         <v>2</v>
       </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
       <c r="E6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>35</v>
       </c>
@@ -682,7 +685,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -696,7 +699,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -707,26 +710,32 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>38</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
       <c r="E10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>40</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -737,15 +746,18 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>16</v>
       </c>
       <c r="B13">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D13">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -753,7 +765,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -764,15 +776,18 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
         <v>43</v>
       </c>
       <c r="B16">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D16">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -780,15 +795,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
         <v>18</v>
       </c>
       <c r="B18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="D18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -796,7 +814,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -804,7 +822,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
         <v>44</v>
       </c>
@@ -812,7 +830,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
         <v>45</v>
       </c>
@@ -820,18 +838,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
         <v>21</v>
       </c>
       <c r="B23">
         <v>2</v>
       </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
       <c r="E23" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -845,7 +866,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -856,7 +877,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -867,7 +888,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -878,7 +899,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -889,18 +910,21 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A29" t="s">
         <v>28</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
       <c r="E29" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -908,7 +932,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -916,7 +940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -927,7 +951,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A33" t="s">
         <v>2</v>
       </c>
@@ -937,25 +961,25 @@
       </c>
       <c r="D33">
         <f>SUM(D3:D32)</f>
-        <v>7.5</v>
+        <v>14.5</v>
       </c>
       <c r="E33" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A44" s="2"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A54" s="2"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="D55" s="1"/>

</xml_diff>

<commit_message>
user input for position limits (not implemented) and use of references
</commit_message>
<xml_diff>
--- a/Project_Grading_Rubric_Checklist.xlsx
+++ b/Project_Grading_Rubric_Checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AERSP 424 Local\Project\AERSP424_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07501A3C-C1CD-454D-AD7B-69CAC61807CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3C97923-3111-4B10-84F1-6A3DEE9ADA3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27810" yWindow="7680" windowWidth="23280" windowHeight="13155" xr2:uid="{E08E36A2-DE9E-42A5-A6DD-8188537D7612}"/>
+    <workbookView xWindow="-27045" yWindow="8445" windowWidth="23280" windowHeight="13155" xr2:uid="{E08E36A2-DE9E-42A5-A6DD-8188537D7612}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -582,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51F30247-08F3-4D53-8CE2-96A4DCDF6914}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -813,6 +813,9 @@
       <c r="B19">
         <v>1</v>
       </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
@@ -961,7 +964,7 @@
       </c>
       <c r="D33">
         <f>SUM(D3:D32)</f>
-        <v>14.5</v>
+        <v>15.5</v>
       </c>
       <c r="E33" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
all primitive types added, rearranging of draft class
</commit_message>
<xml_diff>
--- a/Project_Grading_Rubric_Checklist.xlsx
+++ b/Project_Grading_Rubric_Checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AERSP 424 Local\Project\AERSP424_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3C97923-3111-4B10-84F1-6A3DEE9ADA3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{102D70CC-A638-4684-BCB6-8B588C473338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27045" yWindow="8445" windowWidth="23280" windowHeight="13155" xr2:uid="{E08E36A2-DE9E-42A5-A6DD-8188537D7612}"/>
+    <workbookView xWindow="-26205" yWindow="9120" windowWidth="23280" windowHeight="13155" xr2:uid="{E08E36A2-DE9E-42A5-A6DD-8188537D7612}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -582,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51F30247-08F3-4D53-8CE2-96A4DCDF6914}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -742,6 +742,9 @@
       <c r="B12">
         <v>0.5</v>
       </c>
+      <c r="D12">
+        <v>0.5</v>
+      </c>
       <c r="E12" t="s">
         <v>52</v>
       </c>
@@ -849,7 +852,7 @@
         <v>2</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E23" t="s">
         <v>48</v>
@@ -876,6 +879,9 @@
       <c r="B25">
         <v>2</v>
       </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
       <c r="E25" t="s">
         <v>49</v>
       </c>
@@ -964,7 +970,7 @@
       </c>
       <c r="D33">
         <f>SUM(D3:D32)</f>
-        <v>15.5</v>
+        <v>18</v>
       </c>
       <c r="E33" t="s">
         <v>33</v>

</xml_diff>

<commit_message>
tried to create derived class of the league to create a custom league
</commit_message>
<xml_diff>
--- a/Project_Grading_Rubric_Checklist.xlsx
+++ b/Project_Grading_Rubric_Checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AERSP 424 Local\Project\AERSP424_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{102D70CC-A638-4684-BCB6-8B588C473338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF339E5A-EC17-4F97-804E-57AC9A24E1DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26205" yWindow="9120" windowWidth="23280" windowHeight="13155" xr2:uid="{E08E36A2-DE9E-42A5-A6DD-8188537D7612}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" xr2:uid="{E08E36A2-DE9E-42A5-A6DD-8188537D7612}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -116,9 +116,6 @@
     <t>Inheritance</t>
   </si>
   <si>
-    <t>0 - no classes, 1 - two or less inheritance, More than two inheritance</t>
-  </si>
-  <si>
     <t>Virtual Function / Overriding</t>
   </si>
   <si>
@@ -201,6 +198,9 @@
   </si>
   <si>
     <t>Grade We Think We Will Get</t>
+  </si>
+  <si>
+    <t>0 - no classes, 1 - two or less inheritance, 2 - More than two inheritance</t>
   </si>
 </sst>
 </file>
@@ -582,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51F30247-08F3-4D53-8CE2-96A4DCDF6914}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -609,7 +609,7 @@
         <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>5</v>
@@ -640,7 +640,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.5">
@@ -654,7 +654,7 @@
         <v>1</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.5">
@@ -673,16 +673,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7" t="s">
         <v>35</v>
-      </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.5">
@@ -696,7 +696,7 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.5">
@@ -712,21 +712,21 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
         <v>38</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -746,7 +746,7 @@
         <v>0.5</v>
       </c>
       <c r="E12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.5">
@@ -762,7 +762,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B14">
         <v>0.5</v>
@@ -770,7 +770,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B15">
         <v>0.5</v>
@@ -781,7 +781,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B16">
         <v>0.5</v>
@@ -797,6 +797,9 @@
       <c r="B17">
         <v>1</v>
       </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
@@ -830,7 +833,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -838,7 +841,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B22">
         <v>1</v>
@@ -855,7 +858,7 @@
         <v>2</v>
       </c>
       <c r="E23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.5">
@@ -869,7 +872,7 @@
         <v>2</v>
       </c>
       <c r="E24" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.5">
@@ -883,7 +886,7 @@
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.5">
@@ -894,7 +897,7 @@
         <v>2</v>
       </c>
       <c r="E26" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.5">
@@ -905,45 +908,48 @@
         <v>2</v>
       </c>
       <c r="E27" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28">
         <v>2</v>
       </c>
       <c r="E28" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29" t="s">
         <v>28</v>
-      </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-      <c r="D29">
-        <v>1</v>
-      </c>
-      <c r="E29" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30">
+        <v>0.5</v>
+      </c>
+      <c r="D30">
         <v>0.5</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -951,13 +957,13 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32">
         <v>2.5</v>
       </c>
       <c r="E32" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.5">
@@ -970,10 +976,10 @@
       </c>
       <c r="D33">
         <f>SUM(D3:D32)</f>
-        <v>18</v>
+        <v>19.5</v>
       </c>
       <c r="E33" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.5">

</xml_diff>

<commit_message>
fixed derived class and tried bitwise operator
</commit_message>
<xml_diff>
--- a/Project_Grading_Rubric_Checklist.xlsx
+++ b/Project_Grading_Rubric_Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AERSP 424 Local\Project\AERSP424_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF339E5A-EC17-4F97-804E-57AC9A24E1DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F70F71D2-3C4C-4EE6-9BB9-F5D3967D82E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" xr2:uid="{E08E36A2-DE9E-42A5-A6DD-8188537D7612}"/>
   </bookViews>
@@ -207,7 +207,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -238,13 +238,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -259,13 +272,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -582,8 +598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51F30247-08F3-4D53-8CE2-96A4DCDF6914}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -706,6 +722,9 @@
       <c r="B9">
         <v>1</v>
       </c>
+      <c r="D9" s="5">
+        <v>1</v>
+      </c>
       <c r="E9" t="s">
         <v>14</v>
       </c>
@@ -896,6 +915,9 @@
       <c r="B26">
         <v>2</v>
       </c>
+      <c r="D26" s="5">
+        <v>1</v>
+      </c>
       <c r="E26" t="s">
         <v>46</v>
       </c>
@@ -907,6 +929,9 @@
       <c r="B27">
         <v>2</v>
       </c>
+      <c r="D27" s="6">
+        <v>1</v>
+      </c>
       <c r="E27" t="s">
         <v>54</v>
       </c>
@@ -918,6 +943,9 @@
       <c r="B28">
         <v>2</v>
       </c>
+      <c r="D28">
+        <v>2</v>
+      </c>
       <c r="E28" t="s">
         <v>49</v>
       </c>
@@ -954,6 +982,9 @@
       <c r="B31">
         <v>1</v>
       </c>
+      <c r="D31" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A32" t="s">
@@ -962,6 +993,9 @@
       <c r="B32">
         <v>2.5</v>
       </c>
+      <c r="D32" s="5">
+        <v>1</v>
+      </c>
       <c r="E32" t="s">
         <v>52</v>
       </c>
@@ -976,11 +1010,14 @@
       </c>
       <c r="D33">
         <f>SUM(D3:D32)</f>
-        <v>19.5</v>
+        <v>26.5</v>
       </c>
       <c r="E33" t="s">
         <v>32</v>
       </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A36" s="4"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A44" s="2"/>

</xml_diff>

<commit_message>
added randomizer to robot picks to have high school level math
</commit_message>
<xml_diff>
--- a/Project_Grading_Rubric_Checklist.xlsx
+++ b/Project_Grading_Rubric_Checklist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AERSP 424 Local\Project\AERSP424_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjgly\Downloads\Spring 2024\AERSP 424\Final Project\AERSP424_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F70F71D2-3C4C-4EE6-9BB9-F5D3967D82E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FBF9EA6-7182-41C5-B26B-4B65601FC96C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" xr2:uid="{E08E36A2-DE9E-42A5-A6DD-8188537D7612}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{E08E36A2-DE9E-42A5-A6DD-8188537D7612}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
   <si>
     <t>Checklist</t>
   </si>
@@ -201,6 +201,9 @@
   </si>
   <si>
     <t>0 - no classes, 1 - two or less inheritance, 2 - More than two inheritance</t>
+  </si>
+  <si>
+    <t>double check</t>
   </si>
 </sst>
 </file>
@@ -246,7 +249,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -256,6 +259,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -272,7 +281,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -282,6 +291,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -598,23 +608,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51F30247-08F3-4D53-8CE2-96A4DCDF6914}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="43.64453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.87890625" customWidth="1"/>
-    <col min="5" max="5" width="255.52734375" customWidth="1"/>
+    <col min="1" max="1" width="43.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.90625" customWidth="1"/>
+    <col min="5" max="5" width="255.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -631,7 +641,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -645,7 +655,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -659,7 +669,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -673,7 +683,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -681,13 +691,13 @@
         <v>2</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -701,7 +711,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -715,21 +725,19 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>13</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
-      <c r="D9" s="5">
-        <v>1</v>
-      </c>
+      <c r="D9" s="5"/>
       <c r="E9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -743,7 +751,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -754,7 +762,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -768,7 +776,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -779,7 +787,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -787,7 +795,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -798,7 +806,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -809,18 +817,21 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>17</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
-      <c r="D17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="D17" s="7">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -831,7 +842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -842,7 +853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -850,7 +861,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -858,7 +869,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>44</v>
       </c>
@@ -866,7 +877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -880,7 +891,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -894,7 +905,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -908,35 +919,35 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>24</v>
       </c>
       <c r="B26">
         <v>2</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D26" s="6">
         <v>1</v>
       </c>
       <c r="E26" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>25</v>
       </c>
       <c r="B27">
         <v>2</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D27">
         <v>1</v>
       </c>
       <c r="E27" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -950,7 +961,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -964,7 +975,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -975,32 +986,28 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>30</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
-      <c r="D31" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="D31" s="5"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>31</v>
       </c>
       <c r="B32">
         <v>2.5</v>
       </c>
-      <c r="D32" s="5">
-        <v>1</v>
-      </c>
+      <c r="D32" s="5"/>
       <c r="E32" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>2</v>
       </c>
@@ -1010,28 +1017,28 @@
       </c>
       <c r="D33">
         <f>SUM(D3:D32)</f>
-        <v>26.5</v>
+        <v>24.5</v>
       </c>
       <c r="E33" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="4"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="2"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="2"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="D55" s="1"/>

</xml_diff>

<commit_message>
added error handling and one additional thread
</commit_message>
<xml_diff>
--- a/Project_Grading_Rubric_Checklist.xlsx
+++ b/Project_Grading_Rubric_Checklist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pjgly\Downloads\Spring 2024\AERSP 424\Final Project\AERSP424_Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AERSP 424 Local\Project\AERSP424_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FBF9EA6-7182-41C5-B26B-4B65601FC96C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9609DB51-DD93-4518-B7CD-A489F2A3D00B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{E08E36A2-DE9E-42A5-A6DD-8188537D7612}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" xr2:uid="{E08E36A2-DE9E-42A5-A6DD-8188537D7612}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -281,7 +281,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -290,7 +290,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -608,23 +607,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51F30247-08F3-4D53-8CE2-96A4DCDF6914}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="43.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.90625" customWidth="1"/>
-    <col min="5" max="5" width="255.54296875" customWidth="1"/>
+    <col min="1" max="1" width="43.64453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.87890625" customWidth="1"/>
+    <col min="5" max="5" width="255.52734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -641,7 +640,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -655,7 +654,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -669,7 +668,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -683,7 +682,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -697,7 +696,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -711,7 +710,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -725,7 +724,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -737,7 +736,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -751,7 +750,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -762,7 +761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -776,7 +775,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -787,7 +786,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
         <v>40</v>
       </c>
@@ -795,7 +794,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -806,7 +805,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
         <v>42</v>
       </c>
@@ -817,21 +816,21 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
         <v>17</v>
       </c>
       <c r="B17">
         <v>1</v>
       </c>
-      <c r="D17" s="7">
+      <c r="D17" s="6">
         <v>1</v>
       </c>
       <c r="E17" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -842,7 +841,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -853,7 +852,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -861,7 +860,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -869,7 +868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
         <v>44</v>
       </c>
@@ -877,7 +876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -891,7 +890,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -905,7 +904,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -919,21 +918,21 @@
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A26" t="s">
         <v>24</v>
       </c>
       <c r="B26">
         <v>2</v>
       </c>
-      <c r="D26" s="6">
+      <c r="D26">
         <v>1</v>
       </c>
       <c r="E26" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -947,7 +946,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -961,7 +960,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -975,7 +974,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -986,7 +985,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -995,19 +994,21 @@
       </c>
       <c r="D31" s="5"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A32" t="s">
         <v>31</v>
       </c>
       <c r="B32">
         <v>2.5</v>
       </c>
-      <c r="D32" s="5"/>
+      <c r="D32" s="5">
+        <v>1</v>
+      </c>
       <c r="E32" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A33" t="s">
         <v>2</v>
       </c>
@@ -1017,28 +1018,28 @@
       </c>
       <c r="D33">
         <f>SUM(D3:D32)</f>
-        <v>24.5</v>
+        <v>25.5</v>
       </c>
       <c r="E33" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A36" s="4"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A44" s="2"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A54" s="2"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="D55" s="1"/>

</xml_diff>

<commit_message>
added a lambda function to simplify code
</commit_message>
<xml_diff>
--- a/Project_Grading_Rubric_Checklist.xlsx
+++ b/Project_Grading_Rubric_Checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AERSP 424 Local\Project\AERSP424_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9609DB51-DD93-4518-B7CD-A489F2A3D00B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A93BA90F-82E6-4E0B-9448-E050EE32CC2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" xr2:uid="{E08E36A2-DE9E-42A5-A6DD-8188537D7612}"/>
+    <workbookView xWindow="-26895" yWindow="8385" windowWidth="24930" windowHeight="13635" xr2:uid="{E08E36A2-DE9E-42A5-A6DD-8188537D7612}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>Checklist</t>
   </si>
@@ -204,6 +204,9 @@
   </si>
   <si>
     <t>double check</t>
+  </si>
+  <si>
+    <t>Added one lambda function</t>
   </si>
 </sst>
 </file>
@@ -607,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51F30247-08F3-4D53-8CE2-96A4DCDF6914}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -867,6 +870,12 @@
       <c r="B21">
         <v>1</v>
       </c>
+      <c r="D21">
+        <v>0.5</v>
+      </c>
+      <c r="E21" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
@@ -1018,7 +1027,7 @@
       </c>
       <c r="D33">
         <f>SUM(D3:D32)</f>
-        <v>25.5</v>
+        <v>26</v>
       </c>
       <c r="E33" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Fixed functionality and added function overloading
</commit_message>
<xml_diff>
--- a/Project_Grading_Rubric_Checklist.xlsx
+++ b/Project_Grading_Rubric_Checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AERSP 424 Local\Project\AERSP424_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF220AB-8934-4372-845D-1E0FEFE57C0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BFF1C81-E3E0-49B0-A558-811DBA5C84F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28515" yWindow="9810" windowWidth="27675" windowHeight="13980" xr2:uid="{E08E36A2-DE9E-42A5-A6DD-8188537D7612}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" xr2:uid="{E08E36A2-DE9E-42A5-A6DD-8188537D7612}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>Checklist</t>
   </si>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t>Added two lambda functions</t>
+  </si>
+  <si>
+    <t>added one to the draft class</t>
   </si>
 </sst>
 </file>
@@ -610,8 +613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51F30247-08F3-4D53-8CE2-96A4DCDF6914}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -862,6 +865,12 @@
       <c r="B20">
         <v>0.5</v>
       </c>
+      <c r="D20">
+        <v>0.5</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
@@ -1027,7 +1036,7 @@
       </c>
       <c r="D33">
         <f>SUM(D3:D32)</f>
-        <v>26.5</v>
+        <v>27</v>
       </c>
       <c r="E33" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Three objects per class, also fixed file names
</commit_message>
<xml_diff>
--- a/Project_Grading_Rubric_Checklist.xlsx
+++ b/Project_Grading_Rubric_Checklist.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AERSP 424 Local\Project\AERSP424_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BFF1C81-E3E0-49B0-A558-811DBA5C84F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C90A8C2-23E6-46C6-869F-4103BC7A2187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" xr2:uid="{E08E36A2-DE9E-42A5-A6DD-8188537D7612}"/>
+    <workbookView xWindow="733" yWindow="733" windowWidth="19200" windowHeight="9980" xr2:uid="{E08E36A2-DE9E-42A5-A6DD-8188537D7612}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -613,8 +613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51F30247-08F3-4D53-8CE2-96A4DCDF6914}">
   <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -930,7 +930,7 @@
         <v>2</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E25" t="s">
         <v>48</v>
@@ -1010,7 +1010,9 @@
       <c r="B31">
         <v>1</v>
       </c>
-      <c r="D31" s="5"/>
+      <c r="D31" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A32" t="s">
@@ -1036,7 +1038,7 @@
       </c>
       <c r="D33">
         <f>SUM(D3:D32)</f>
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E33" t="s">
         <v>32</v>

</xml_diff>